<commit_message>
descrevendo as equações do modelo
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/dados_calibracao.xlsx
+++ b/models/dissertation-model/modelo-R/dados_calibracao.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">time</t>
   </si>
   <si>
     <t xml:space="preserve">fIndustryOrderRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sPrice1</t>
   </si>
 </sst>
 </file>
@@ -123,17 +126,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -143,6 +146,9 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -151,8 +157,11 @@
       <c r="B2" s="0" t="n">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <f aca="false">A2+1</f>
         <v>1</v>
@@ -160,8 +169,12 @@
       <c r="B3" s="0" t="n">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="n">
+        <f aca="false">C2</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <f aca="false">A3+1</f>
         <v>2</v>
@@ -169,8 +182,12 @@
       <c r="B4" s="0" t="n">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="n">
+        <f aca="false">C3</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <f aca="false">A4+1</f>
         <v>3</v>
@@ -178,8 +195,12 @@
       <c r="B5" s="0" t="n">
         <v>355</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="n">
+        <f aca="false">C4</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <f aca="false">A5+1</f>
         <v>4</v>
@@ -187,8 +208,12 @@
       <c r="B6" s="0" t="n">
         <v>1816</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="n">
+        <f aca="false">C5</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <f aca="false">A6+1</f>
         <v>5</v>
@@ -196,8 +221,12 @@
       <c r="B7" s="0" t="n">
         <v>5978</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="n">
+        <f aca="false">C6</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <f aca="false">A7+1</f>
         <v>6</v>
@@ -205,8 +234,12 @@
       <c r="B8" s="0" t="n">
         <v>24265</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="n">
+        <f aca="false">C7</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <f aca="false">A8+1</f>
         <v>7</v>
@@ -214,8 +247,12 @@
       <c r="B9" s="0" t="n">
         <v>35508</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="n">
+        <f aca="false">C8</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <f aca="false">A9+1</f>
         <v>8</v>
@@ -223,8 +260,12 @@
       <c r="B10" s="0" t="n">
         <v>72503</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="n">
+        <f aca="false">C9</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <f aca="false">A10+1</f>
         <v>9</v>
@@ -232,14 +273,22 @@
       <c r="B11" s="0" t="n">
         <v>139584</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="n">
+        <f aca="false">C10</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <f aca="false">A11+1</f>
         <v>10</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>232336</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <f aca="false">C11</f>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lista de parâmetros no excel
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/dados_calibracao.xlsx
+++ b/models/dissertation-model/modelo-R/dados_calibracao.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" state="visible" r:id="rId2"/>
@@ -129,14 +129,14 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
alteracoes para calibração do modelo - impressoras industriais
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/dados_calibracao.xlsx
+++ b/models/dissertation-model/modelo-R/dados_calibracao.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="66">
   <si>
     <t>time</t>
   </si>
@@ -169,9 +169,6 @@
     <t>http://wohlersassociates.com/blog/2016/01/popularity-of-fdm/</t>
   </si>
   <si>
-    <t>Receitas em Milhões de Dólares - Sistemas</t>
-  </si>
-  <si>
     <t>Patentes Concedidas</t>
   </si>
   <si>
@@ -215,6 +212,21 @@
   </si>
   <si>
     <t>Período dede 88: http://docplayer.net/9034750-Executive-summary-wohlers-report-rapid-prototyping-tooling-state-of-the-industry-annual-worldwide-progress-report.html</t>
+  </si>
+  <si>
+    <t>Preços Impressoras Pessoais</t>
+  </si>
+  <si>
+    <t>Preços Impressoras Industriais</t>
+  </si>
+  <si>
+    <t>ReferencePrice</t>
+  </si>
+  <si>
+    <t>ReferenceIndustryDemandElasticity</t>
+  </si>
+  <si>
+    <t>IndustryShipmentsReference</t>
   </si>
 </sst>
 </file>
@@ -265,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -279,6 +291,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -769,24 +784,104 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC801FAE-43CD-4D0B-B936-19396D7BF964}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
       <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3500</v>
+      </c>
+      <c r="B2">
+        <v>20000</v>
+      </c>
+      <c r="C2">
+        <f>A2*1000</f>
+        <v>3500000</v>
+      </c>
+      <c r="D2">
+        <v>0.2</v>
+      </c>
+      <c r="E2">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>5050</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>6100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>7771</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>10310.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>12850</v>
       </c>
     </row>
   </sheetData>
@@ -796,30 +891,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA85A1AB-9274-4FF5-A00A-BBD9450F0BFF}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="9" width="40" style="1" customWidth="1"/>
-    <col min="10" max="10" width="43.5703125" customWidth="1"/>
-    <col min="11" max="11" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="39.140625" customWidth="1"/>
-    <col min="13" max="13" width="41.140625" customWidth="1"/>
+    <col min="2" max="10" width="40" style="1" customWidth="1"/>
+    <col min="11" max="11" width="43.5703125" customWidth="1"/>
+    <col min="12" max="12" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.140625" customWidth="1"/>
+    <col min="14" max="14" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -830,34 +925,37 @@
         <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>36</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -871,23 +969,21 @@
         <v>7</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" t="s">
         <v>10</v>
-      </c>
-      <c r="K3" t="s">
-        <v>35</v>
       </c>
       <c r="L3" t="s">
         <v>35</v>
@@ -895,8 +991,11 @@
       <c r="M3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -904,18 +1003,16 @@
         <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>18</v>
@@ -923,25 +1020,28 @@
       <c r="M4" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ref="A6:A8" si="0">A7-1</f>
         <v>1988</v>
@@ -949,12 +1049,12 @@
       <c r="D6" s="1">
         <v>34</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="1"/>
+      <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1989</v>
@@ -962,12 +1062,12 @@
       <c r="D7" s="1">
         <v>104</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="1"/>
+      <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1990</v>
@@ -975,12 +1075,12 @@
       <c r="D8" s="1">
         <v>114</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="1"/>
+      <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ref="A9:A16" si="1">A10-1</f>
         <v>1991</v>
@@ -988,12 +1088,12 @@
       <c r="D9" s="1">
         <v>82</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="1"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>1992</v>
@@ -1001,12 +1101,12 @@
       <c r="D10" s="1">
         <v>111</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="1"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>1993</v>
@@ -1014,12 +1114,12 @@
       <c r="D11" s="1">
         <v>157</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="1"/>
+      <c r="K11" s="2"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>1994</v>
@@ -1027,12 +1127,12 @@
       <c r="D12" s="1">
         <v>320</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="1"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>1995</v>
@@ -1040,12 +1140,12 @@
       <c r="D13" s="1">
         <v>523</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="1"/>
+      <c r="K13" s="2"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>1996</v>
@@ -1053,12 +1153,12 @@
       <c r="D14" s="1">
         <v>790</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="1"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>1997</v>
@@ -1066,12 +1166,12 @@
       <c r="D15" s="1">
         <v>1040</v>
       </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="1"/>
+      <c r="K15" s="2"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>1998</v>
@@ -1079,22 +1179,26 @@
       <c r="D16" s="1">
         <v>982</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="1"/>
+      <c r="K16" s="2"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>A18-1</f>
         <v>1999</v>
       </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="1"/>
+      <c r="D17" s="7">
+        <f>AVERAGE(D16,D18)</f>
+        <v>1091</v>
+      </c>
+      <c r="K17" s="2"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2000</v>
       </c>
@@ -1104,21 +1208,21 @@
       <c r="D18" s="1">
         <v>1200</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>103</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>140</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <f>9145/4015</f>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I18" s="5">
+      <c r="J18" s="5">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2001</v>
       </c>
@@ -1128,21 +1232,21 @@
       <c r="D19" s="1">
         <v>1200</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>100</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>160</v>
       </c>
-      <c r="H19" s="1">
-        <f t="shared" ref="H19:H35" si="2">9145/4015</f>
+      <c r="I19" s="1">
+        <f t="shared" ref="I19:I35" si="2">9145/4015</f>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I19" s="5">
+      <c r="J19" s="5">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2002</v>
       </c>
@@ -1152,21 +1256,21 @@
       <c r="D20" s="1">
         <v>1400</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>140</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>202</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I20" s="5">
+      <c r="J20" s="5">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2003</v>
       </c>
@@ -1176,24 +1280,24 @@
       <c r="D21" s="1">
         <v>1800</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>180</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>240</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I21" s="5">
+      <c r="J21" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J21" s="3">
+      <c r="K21" s="3">
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2004</v>
       </c>
@@ -1203,24 +1307,24 @@
       <c r="D22" s="1">
         <v>2600</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>199</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>298</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I22" s="5">
+      <c r="J22" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J22" s="3">
+      <c r="K22" s="3">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2005</v>
       </c>
@@ -1230,24 +1334,24 @@
       <c r="D23" s="1">
         <v>3500</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>220</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>350</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I23" s="5">
+      <c r="J23" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J23" s="3">
+      <c r="K23" s="3">
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2006</v>
       </c>
@@ -1257,24 +1361,24 @@
       <c r="D24" s="1">
         <v>4000</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>210</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>345</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I24" s="5">
+      <c r="J24" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J24" s="3">
+      <c r="K24" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2007</v>
       </c>
@@ -1287,24 +1391,24 @@
       <c r="D25" s="1">
         <v>5000</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>222</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>403</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I25" s="5">
+      <c r="J25" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J25" s="3">
+      <c r="K25" s="3">
         <v>0.11700000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2008</v>
       </c>
@@ -1317,24 +1421,24 @@
       <c r="D26" s="1">
         <v>5050</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>202</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>385</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I26" s="5">
+      <c r="J26" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J26" s="4">
+      <c r="K26" s="4">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2009</v>
       </c>
@@ -1347,24 +1451,24 @@
       <c r="D27" s="1">
         <v>4600</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1">
         <v>202</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <v>398</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I27" s="5">
+      <c r="J27" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J27" s="3">
+      <c r="K27" s="3">
         <v>0.17199999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2010</v>
       </c>
@@ -1377,24 +1481,24 @@
       <c r="D28" s="1">
         <v>6100</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>220</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>480</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I28" s="5">
+      <c r="J28" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J28" s="3">
+      <c r="K28" s="3">
         <v>0.19600000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2011</v>
       </c>
@@ -1407,33 +1511,33 @@
       <c r="D29" s="1">
         <v>6500</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>205</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <v>510</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I29" s="5">
+      <c r="J29" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J29" s="4">
+      <c r="K29" s="4">
         <v>0.24</v>
       </c>
-      <c r="K29" s="4">
+      <c r="L29" s="4">
         <v>0.15</v>
       </c>
-      <c r="L29" s="4">
+      <c r="M29" s="4">
         <v>0.24</v>
       </c>
-      <c r="M29" s="4">
+      <c r="N29" s="4">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2012</v>
       </c>
@@ -1446,33 +1550,33 @@
       <c r="D30" s="1">
         <v>7771</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>210</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>695</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I30" s="5">
+      <c r="J30" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J30" s="3">
+      <c r="K30" s="3">
         <v>0.28299999999999997</v>
       </c>
-      <c r="K30" s="4">
+      <c r="L30" s="4">
         <v>0.22</v>
       </c>
-      <c r="L30" s="4">
+      <c r="M30" s="4">
         <v>0.21</v>
       </c>
-      <c r="M30" s="4">
+      <c r="N30" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2013</v>
       </c>
@@ -1486,24 +1590,26 @@
         <f>AVERAGE(D32,D30)</f>
         <v>10310.5</v>
       </c>
-      <c r="H31" s="1">
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="I31" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I31" s="5">
+      <c r="J31" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="K31" s="4">
+      <c r="L31" s="4">
         <v>0.12</v>
       </c>
-      <c r="L31" s="4">
+      <c r="M31" s="4">
         <v>0.2</v>
       </c>
-      <c r="M31" s="4">
+      <c r="N31" s="4">
         <v>0.16</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2014</v>
       </c>
@@ -1516,86 +1622,86 @@
       <c r="D32" s="1">
         <v>12850</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I32" s="5">
+      <c r="J32" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="K32" s="4">
+      <c r="L32" s="4">
         <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="L32" s="4">
-        <v>0.15</v>
       </c>
       <c r="M32" s="4">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2015</v>
       </c>
       <c r="B33" s="1">
         <v>850</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I33" s="5">
+      <c r="J33" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="K33" s="4">
+      <c r="L33" s="4">
         <v>-0.02</v>
       </c>
-      <c r="L33" s="4">
+      <c r="M33" s="4">
         <v>0.2</v>
       </c>
-      <c r="M33" s="4">
+      <c r="N33" s="4">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2016</v>
       </c>
       <c r="B34" s="1">
         <v>957</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I34" s="5">
+      <c r="J34" s="5">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2017</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <f t="shared" si="2"/>
         <v>2.2777085927770861</v>
       </c>
-      <c r="I35" s="5">
+      <c r="J35" s="5">
         <v>0.55000000000000004</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K4" r:id="rId1" xr:uid="{0AF5EBA6-0D09-45EE-9304-AE82D6A406D7}"/>
-    <hyperlink ref="L4" r:id="rId2" xr:uid="{9FB3392E-F3AB-46C2-B679-926CC38B3FE6}"/>
-    <hyperlink ref="M4" r:id="rId3" xr:uid="{98A08BC3-8B78-4B54-9AAD-71734B66560A}"/>
+    <hyperlink ref="L4" r:id="rId1" xr:uid="{0AF5EBA6-0D09-45EE-9304-AE82D6A406D7}"/>
+    <hyperlink ref="M4" r:id="rId2" xr:uid="{9FB3392E-F3AB-46C2-B679-926CC38B3FE6}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{98A08BC3-8B78-4B54-9AAD-71734B66560A}"/>
     <hyperlink ref="C4" r:id="rId4" xr:uid="{B33AD3C4-DF21-4C70-A92F-ACDB17CF0076}"/>
     <hyperlink ref="D3" r:id="rId5" xr:uid="{ED7BC98D-C10F-4444-BEDE-A4107D18A762}"/>
-    <hyperlink ref="F3" r:id="rId6" xr:uid="{47E562DC-8DDF-4CFC-870A-D01584B10020}"/>
-    <hyperlink ref="G3" r:id="rId7" xr:uid="{844F590C-BFC2-4EBB-94D8-76341685240A}"/>
-    <hyperlink ref="H3" r:id="rId8" xr:uid="{721FDE8F-1977-4299-8EBB-74AEA5A0BB3D}"/>
-    <hyperlink ref="I4" r:id="rId9" display="https://www.slideshare.net/alanek/wohlers-report-2013-executive-summary" xr:uid="{7CE1771F-1B97-4730-8AC0-A70B8DB75065}"/>
-    <hyperlink ref="I3" r:id="rId10" xr:uid="{42E910EE-5196-41D1-BF92-7C8AF466E136}"/>
+    <hyperlink ref="G3" r:id="rId6" xr:uid="{47E562DC-8DDF-4CFC-870A-D01584B10020}"/>
+    <hyperlink ref="H3" r:id="rId7" xr:uid="{844F590C-BFC2-4EBB-94D8-76341685240A}"/>
+    <hyperlink ref="I3" r:id="rId8" xr:uid="{721FDE8F-1977-4299-8EBB-74AEA5A0BB3D}"/>
+    <hyperlink ref="J4" r:id="rId9" display="https://www.slideshare.net/alanek/wohlers-report-2013-executive-summary" xr:uid="{7CE1771F-1B97-4730-8AC0-A70B8DB75065}"/>
+    <hyperlink ref="J3" r:id="rId10" xr:uid="{42E910EE-5196-41D1-BF92-7C8AF466E136}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1606,7 +1712,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,18 +1876,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2">
         <v>92</v>
@@ -1805,7 +1911,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>67</v>
@@ -1813,7 +1919,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6">
         <v>48</v>
@@ -1821,7 +1927,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7">
         <v>41</v>
@@ -1829,7 +1935,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8">
         <v>38</v>
@@ -1837,7 +1943,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <v>36</v>

</xml_diff>